<commit_message>
Fix row group layout extraction
</commit_message>
<xml_diff>
--- a/src/main/processing/Any2Json/examples/ReadIntelliTable2/data/TestBench.xlsx
+++ b/src/main/processing/Any2Json/examples/ReadIntelliTable2/data/TestBench.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRU_SG1\Projects\Any2Json\src\main\processing\Any2Json\examples\ReadIntelliTable2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D6242B-3523-4E6C-A8C4-10E0E7829C57}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35099EBC-7DEB-4C91-88A3-8CD6F25D7B50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1725B7E8-4632-49E5-8EBE-7E29775D2CA9}"/>
   </bookViews>
@@ -624,7 +624,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,8 +637,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF20C69B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -741,11 +759,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,9 +802,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -770,6 +816,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -797,12 +847,48 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF20C69B"/>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1111,22 +1197,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D780D69-5FB2-48CC-9A0C-B58C2902AE10}">
-  <dimension ref="B2:X110"/>
+  <dimension ref="B2:AA110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30:T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C2" s="18">
+      <c r="C2" s="21">
         <v>43617</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -1197,60 +1283,60 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="P8" s="13" t="s">
+      <c r="P8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
     </row>
     <row r="9" spans="2:24" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="P9" s="15" t="s">
+      <c r="P9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="15" t="s">
+      <c r="Q9" s="19"/>
+      <c r="R9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="S9" s="17"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="15" t="s">
+      <c r="S9" s="20"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="V9" s="17"/>
-      <c r="W9" s="16"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="19"/>
       <c r="X9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="10" t="s">
+      <c r="Q10" s="15"/>
+      <c r="R10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="11"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="10" t="s">
+      <c r="S10" s="14"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="V10" s="11"/>
-      <c r="W10" s="12"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="15"/>
       <c r="X10" s="3">
         <v>1</v>
       </c>
@@ -1259,2979 +1345,2983 @@
       <c r="B11" t="s">
         <v>116</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="10" t="s">
+      <c r="Q11" s="15"/>
+      <c r="R11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="S11" s="11"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="10" t="s">
+      <c r="S11" s="14"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="V11" s="11"/>
-      <c r="W11" s="12"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="15"/>
       <c r="X11" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="P12" s="10" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="P12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="10" t="s">
+      <c r="Q12" s="15"/>
+      <c r="R12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S12" s="11"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="10" t="s">
+      <c r="S12" s="14"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="V12" s="11"/>
-      <c r="W12" s="12"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="15"/>
       <c r="X12" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:24" ht="51" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="K13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="P13" s="10" t="s">
+      <c r="P13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="10" t="s">
+      <c r="Q13" s="15"/>
+      <c r="R13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="S13" s="11"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="10" t="s">
+      <c r="S13" s="14"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="V13" s="11"/>
-      <c r="W13" s="12"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="15"/>
       <c r="X13" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <f>ROW()-3</f>
         <v>11</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>167721</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>12732</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="7">
         <v>2</v>
       </c>
-      <c r="L14" s="8"/>
-      <c r="P14" s="10" t="s">
+      <c r="L14" s="7"/>
+      <c r="P14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="10" t="s">
+      <c r="Q14" s="15"/>
+      <c r="R14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="S14" s="11"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="10" t="s">
+      <c r="S14" s="14"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V14" s="11"/>
-      <c r="W14" s="12"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="15"/>
       <c r="X14" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <f t="shared" ref="B15:B34" si="0">ROW()-3</f>
         <v>12</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>167721</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>18646</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K15" s="8">
-        <v>1</v>
-      </c>
-      <c r="L15" s="8"/>
-      <c r="P15" s="10" t="s">
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="P15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="10" t="s">
+      <c r="Q15" s="15"/>
+      <c r="R15" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="S15" s="11"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="10" t="s">
+      <c r="S15" s="14"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="V15" s="11"/>
-      <c r="W15" s="12"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="15"/>
       <c r="X15" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>167721</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="7">
         <v>21539</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16" s="7">
         <v>3</v>
       </c>
-      <c r="L16" s="8"/>
-      <c r="P16" s="10" t="s">
+      <c r="L16" s="7"/>
+      <c r="P16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="10" t="s">
+      <c r="Q16" s="15"/>
+      <c r="R16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="S16" s="11"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="10" t="s">
+      <c r="S16" s="14"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="V16" s="11"/>
-      <c r="W16" s="12"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="15"/>
       <c r="X16" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>167721</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>23165</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17" s="7">
         <v>4</v>
       </c>
-      <c r="L17" s="8"/>
-      <c r="P17" s="10" t="s">
+      <c r="L17" s="7"/>
+      <c r="P17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="10" t="s">
+      <c r="Q17" s="15"/>
+      <c r="R17" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S17" s="11"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="10" t="s">
+      <c r="S17" s="14"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V17" s="11"/>
-      <c r="W17" s="12"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="15"/>
       <c r="X17" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>167721</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <v>23293</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K18" s="8">
-        <v>1</v>
-      </c>
-      <c r="L18" s="8"/>
-      <c r="P18" s="10" t="s">
+      <c r="K18" s="7">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="P18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="10" t="s">
+      <c r="Q18" s="15"/>
+      <c r="R18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="S18" s="11"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="10" t="s">
+      <c r="S18" s="14"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="V18" s="11"/>
-      <c r="W18" s="12"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="15"/>
       <c r="X18" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="8">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>167721</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <v>45676</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K19" s="8">
-        <v>1</v>
-      </c>
-      <c r="L19" s="8"/>
-      <c r="P19" s="10" t="s">
+      <c r="K19" s="7">
+        <v>1</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="P19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="10" t="s">
+      <c r="Q19" s="15"/>
+      <c r="R19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="S19" s="11"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="10" t="s">
+      <c r="S19" s="14"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="V19" s="11"/>
-      <c r="W19" s="12"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="15"/>
       <c r="X19" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="8">
+      <c r="AA19" s="11"/>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>167721</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>43375</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K20" s="8">
-        <v>1</v>
-      </c>
-      <c r="L20" s="8"/>
-      <c r="P20" s="10" t="s">
+      <c r="K20" s="7">
+        <v>1</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="P20" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="Q20" s="12"/>
-      <c r="R20" s="10" t="s">
+      <c r="Q20" s="15"/>
+      <c r="R20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="S20" s="11"/>
-      <c r="T20" s="12"/>
-      <c r="U20" s="10" t="s">
+      <c r="S20" s="14"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="V20" s="11"/>
-      <c r="W20" s="12"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="15"/>
       <c r="X20" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="8">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B21" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>167721</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>22567</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K21" s="8">
-        <v>1</v>
-      </c>
-      <c r="L21" s="8"/>
-      <c r="P21" s="10" t="s">
+      <c r="K21" s="7">
+        <v>1</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="P21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="10" t="s">
+      <c r="Q21" s="15"/>
+      <c r="R21" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="S21" s="11"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="10" t="s">
+      <c r="S21" s="14"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="V21" s="11"/>
-      <c r="W21" s="12"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="15"/>
       <c r="X21" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="8">
+      <c r="Z21" s="10"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B22" s="7">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>167721</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="7">
         <v>959</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22" s="7">
         <v>4</v>
       </c>
-      <c r="L22" s="8"/>
-      <c r="P22" s="10" t="s">
+      <c r="L22" s="7"/>
+      <c r="P22" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="10" t="s">
+      <c r="Q22" s="15"/>
+      <c r="R22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S22" s="11"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="10" t="s">
+      <c r="S22" s="14"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="V22" s="11"/>
-      <c r="W22" s="12"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="15"/>
       <c r="X22" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="8">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B23" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>167721</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="7">
         <v>24257</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K23" s="8">
-        <v>1</v>
-      </c>
-      <c r="L23" s="8"/>
-      <c r="P23" s="10" t="s">
+      <c r="K23" s="7">
+        <v>1</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="P23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="Q23" s="12"/>
-      <c r="R23" s="10" t="s">
+      <c r="Q23" s="15"/>
+      <c r="R23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="S23" s="11"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="10" t="s">
+      <c r="S23" s="14"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="V23" s="11"/>
-      <c r="W23" s="12"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="15"/>
       <c r="X23" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="8">
+      <c r="AA23" s="12"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B24" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>167721</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <v>1311</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="7">
         <v>3</v>
       </c>
-      <c r="L24" s="8"/>
-      <c r="P24" s="10" t="s">
+      <c r="L24" s="7"/>
+      <c r="P24" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="Q24" s="12"/>
-      <c r="R24" s="10" t="s">
+      <c r="Q24" s="30"/>
+      <c r="R24" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="S24" s="11"/>
-      <c r="T24" s="12"/>
-      <c r="U24" s="10" t="s">
+      <c r="S24" s="31"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="V24" s="11"/>
-      <c r="W24" s="12"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="30"/>
       <c r="X24" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="8">
+    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="7">
         <v>167721</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>20910</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K25" s="8">
-        <v>1</v>
-      </c>
-      <c r="L25" s="8"/>
-      <c r="P25" s="10" t="s">
+      <c r="K25" s="7">
+        <v>1</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="P25" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="3">
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="14"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="29">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="8">
+    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B26" s="7">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>167721</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <v>22029</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="7">
         <v>2</v>
       </c>
-      <c r="L26" s="8"/>
-      <c r="P26" s="4" t="s">
+      <c r="L26" s="7"/>
+      <c r="P26" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="8">
+    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>167721</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>22708</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="7">
         <v>2</v>
       </c>
-      <c r="L27" s="8"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="8">
+      <c r="L27" s="7"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
+      <c r="V27" s="22"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="22"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B28" s="7">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>167721</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>40985</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K28" s="8">
-        <v>1</v>
-      </c>
-      <c r="L28" s="8"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="17"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="2"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="8">
+      <c r="K28" s="7">
+        <v>1</v>
+      </c>
+      <c r="L28" s="7"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="24"/>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B29" s="7">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="7">
         <v>167721</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="7">
         <v>41478</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H29" s="8" t="s">
+      <c r="H29" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="7">
         <v>2</v>
       </c>
-      <c r="L29" s="8"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="10"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="12"/>
-      <c r="X29" s="3"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="8">
+      <c r="L29" s="7"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="25"/>
+      <c r="W29" s="25"/>
+      <c r="X29" s="26"/>
+      <c r="Z29" s="9"/>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B30" s="7">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>167721</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="7">
         <v>41378</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="J30" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K30" s="8">
-        <v>1</v>
-      </c>
-      <c r="L30" s="8"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="12"/>
-      <c r="U30" s="10"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="12"/>
-      <c r="X30" s="3"/>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="8">
+      <c r="K30" s="7">
+        <v>1</v>
+      </c>
+      <c r="L30" s="7"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="25"/>
+      <c r="S30" s="25"/>
+      <c r="T30" s="25"/>
+      <c r="U30" s="25"/>
+      <c r="V30" s="25"/>
+      <c r="W30" s="25"/>
+      <c r="X30" s="26"/>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B31" s="7">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="7">
         <v>167721</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="7">
         <v>28120</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="H31" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="I31" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="J31" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K31" s="8">
-        <v>1</v>
-      </c>
-      <c r="L31" s="8"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="12"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="12"/>
-      <c r="X31" s="3"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B32" s="8">
+      <c r="K31" s="7">
+        <v>1</v>
+      </c>
+      <c r="L31" s="7"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="25"/>
+      <c r="W31" s="25"/>
+      <c r="X31" s="26"/>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B32" s="7">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <v>167721</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="7">
         <v>16617</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K32" s="8">
-        <v>1</v>
-      </c>
-      <c r="L32" s="8"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="12"/>
-      <c r="U32" s="10"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="12"/>
-      <c r="X32" s="3"/>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="L32" s="7"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="25"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="25"/>
+      <c r="V32" s="25"/>
+      <c r="W32" s="25"/>
+      <c r="X32" s="26"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B33" s="8">
+      <c r="B33" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>167721</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="7">
         <v>41866</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K33" s="8">
-        <v>1</v>
-      </c>
-      <c r="L33" s="8"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="12"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="12"/>
-      <c r="X33" s="3"/>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+      <c r="L33" s="7"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="25"/>
+      <c r="S33" s="25"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="25"/>
+      <c r="V33" s="25"/>
+      <c r="W33" s="25"/>
+      <c r="X33" s="26"/>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B34" s="8">
+      <c r="B34" s="7">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>167721</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="7">
         <v>26198</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34" s="7">
         <v>2</v>
       </c>
-      <c r="L34" s="8"/>
-      <c r="P34" s="13" t="s">
+      <c r="L34" s="7"/>
+      <c r="P34" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13"/>
-      <c r="U34" s="13"/>
-      <c r="V34" s="13"/>
-      <c r="W34" s="13"/>
-      <c r="X34" s="13"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="16"/>
     </row>
     <row r="35" spans="2:24" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="P35" s="15" t="s">
+      <c r="P35" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="15" t="s">
+      <c r="Q35" s="19"/>
+      <c r="R35" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="S35" s="17"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="15" t="s">
+      <c r="S35" s="20"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="V35" s="17"/>
-      <c r="W35" s="16"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="19"/>
       <c r="X35" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="P36" s="10" t="s">
+      <c r="P36" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="10" t="s">
+      <c r="Q36" s="15"/>
+      <c r="R36" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="S36" s="11"/>
-      <c r="T36" s="12"/>
-      <c r="U36" s="10" t="s">
+      <c r="S36" s="14"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="V36" s="11"/>
-      <c r="W36" s="12"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="15"/>
       <c r="X36" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="P37" s="10" t="s">
+      <c r="P37" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="10" t="s">
+      <c r="Q37" s="15"/>
+      <c r="R37" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="S37" s="11"/>
-      <c r="T37" s="12"/>
-      <c r="U37" s="10" t="s">
+      <c r="S37" s="14"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="V37" s="11"/>
-      <c r="W37" s="12"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="15"/>
       <c r="X37" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="P38" s="10" t="s">
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="P38" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q38" s="12"/>
-      <c r="R38" s="10" t="s">
+      <c r="Q38" s="15"/>
+      <c r="R38" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="S38" s="11"/>
-      <c r="T38" s="12"/>
-      <c r="U38" s="10" t="s">
+      <c r="S38" s="14"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="V38" s="11"/>
-      <c r="W38" s="12"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="15"/>
       <c r="X38" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="2:24" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="15" t="s">
+      <c r="D39" s="19"/>
+      <c r="E39" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="15" t="s">
+      <c r="F39" s="20"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I39" s="17"/>
-      <c r="J39" s="16"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="19"/>
       <c r="K39" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P39" s="10" t="s">
+      <c r="P39" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Q39" s="12"/>
-      <c r="R39" s="10" t="s">
+      <c r="Q39" s="15"/>
+      <c r="R39" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="S39" s="11"/>
-      <c r="T39" s="12"/>
-      <c r="U39" s="10" t="s">
+      <c r="S39" s="14"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="V39" s="11"/>
-      <c r="W39" s="12"/>
+      <c r="V39" s="14"/>
+      <c r="W39" s="15"/>
       <c r="X39" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="10" t="s">
+      <c r="D40" s="15"/>
+      <c r="E40" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="10" t="s">
+      <c r="F40" s="14"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I40" s="11"/>
-      <c r="J40" s="12"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="3">
         <v>1</v>
       </c>
-      <c r="P40" s="10" t="s">
+      <c r="P40" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Q40" s="12"/>
-      <c r="R40" s="10" t="s">
+      <c r="Q40" s="15"/>
+      <c r="R40" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="S40" s="11"/>
-      <c r="T40" s="12"/>
-      <c r="U40" s="10" t="s">
+      <c r="S40" s="14"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="V40" s="11"/>
-      <c r="W40" s="12"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="15"/>
       <c r="X40" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="10" t="s">
+      <c r="D41" s="15"/>
+      <c r="E41" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="10" t="s">
+      <c r="F41" s="14"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I41" s="11"/>
-      <c r="J41" s="12"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="15"/>
       <c r="K41" s="3">
         <v>2</v>
       </c>
-      <c r="P41" s="10" t="s">
+      <c r="P41" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="Q41" s="12"/>
-      <c r="R41" s="10" t="s">
+      <c r="Q41" s="15"/>
+      <c r="R41" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="S41" s="11"/>
-      <c r="T41" s="12"/>
-      <c r="U41" s="10" t="s">
+      <c r="S41" s="14"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="V41" s="11"/>
-      <c r="W41" s="12"/>
+      <c r="V41" s="14"/>
+      <c r="W41" s="15"/>
       <c r="X41" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="10" t="s">
+      <c r="D42" s="15"/>
+      <c r="E42" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="10" t="s">
+      <c r="F42" s="14"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I42" s="11"/>
-      <c r="J42" s="12"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="15"/>
       <c r="K42" s="3">
         <v>2</v>
       </c>
-      <c r="P42" s="10" t="s">
+      <c r="P42" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Q42" s="12"/>
-      <c r="R42" s="10" t="s">
+      <c r="Q42" s="15"/>
+      <c r="R42" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="S42" s="11"/>
-      <c r="T42" s="12"/>
-      <c r="U42" s="10" t="s">
+      <c r="S42" s="14"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="V42" s="11"/>
-      <c r="W42" s="12"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="15"/>
       <c r="X42" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="10" t="s">
+      <c r="D43" s="15"/>
+      <c r="E43" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="10" t="s">
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I43" s="11"/>
-      <c r="J43" s="12"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="15"/>
       <c r="K43" s="3">
         <v>1</v>
       </c>
-      <c r="P43" s="10" t="s">
+      <c r="P43" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="10" t="s">
+      <c r="Q43" s="15"/>
+      <c r="R43" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="S43" s="11"/>
-      <c r="T43" s="12"/>
-      <c r="U43" s="10" t="s">
+      <c r="S43" s="14"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="V43" s="11"/>
-      <c r="W43" s="12"/>
+      <c r="V43" s="14"/>
+      <c r="W43" s="15"/>
       <c r="X43" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="10" t="s">
+      <c r="D44" s="15"/>
+      <c r="E44" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="10" t="s">
+      <c r="F44" s="14"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I44" s="11"/>
-      <c r="J44" s="12"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="15"/>
       <c r="K44" s="3">
         <v>1</v>
       </c>
-      <c r="P44" s="10" t="s">
+      <c r="P44" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Q44" s="12"/>
-      <c r="R44" s="10" t="s">
+      <c r="Q44" s="15"/>
+      <c r="R44" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="S44" s="11"/>
-      <c r="T44" s="12"/>
-      <c r="U44" s="10" t="s">
+      <c r="S44" s="14"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="V44" s="11"/>
-      <c r="W44" s="12"/>
+      <c r="V44" s="14"/>
+      <c r="W44" s="15"/>
       <c r="X44" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="10" t="s">
+      <c r="D45" s="15"/>
+      <c r="E45" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="11"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="10" t="s">
+      <c r="F45" s="14"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="I45" s="11"/>
-      <c r="J45" s="12"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="15"/>
       <c r="K45" s="3">
         <v>1</v>
       </c>
-      <c r="P45" s="10" t="s">
+      <c r="P45" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="Q45" s="12"/>
-      <c r="R45" s="10" t="s">
+      <c r="Q45" s="15"/>
+      <c r="R45" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="S45" s="11"/>
-      <c r="T45" s="12"/>
-      <c r="U45" s="10" t="s">
+      <c r="S45" s="14"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="V45" s="11"/>
-      <c r="W45" s="12"/>
+      <c r="V45" s="14"/>
+      <c r="W45" s="15"/>
       <c r="X45" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="10" t="s">
+      <c r="D46" s="15"/>
+      <c r="E46" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="10" t="s">
+      <c r="F46" s="14"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I46" s="11"/>
-      <c r="J46" s="12"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="15"/>
       <c r="K46" s="3">
         <v>1</v>
       </c>
-      <c r="P46" s="10" t="s">
+      <c r="P46" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="Q46" s="12"/>
-      <c r="R46" s="10" t="s">
+      <c r="Q46" s="15"/>
+      <c r="R46" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="S46" s="11"/>
-      <c r="T46" s="12"/>
-      <c r="U46" s="10" t="s">
+      <c r="S46" s="14"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="V46" s="11"/>
-      <c r="W46" s="12"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="15"/>
       <c r="X46" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="10" t="s">
+      <c r="D47" s="15"/>
+      <c r="E47" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="10" t="s">
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="15"/>
       <c r="K47" s="3">
         <v>1</v>
       </c>
-      <c r="P47" s="10" t="s">
+      <c r="P47" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Q47" s="12"/>
-      <c r="R47" s="10" t="s">
+      <c r="Q47" s="15"/>
+      <c r="R47" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="S47" s="11"/>
-      <c r="T47" s="12"/>
-      <c r="U47" s="10" t="s">
+      <c r="S47" s="14"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="V47" s="11"/>
-      <c r="W47" s="12"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="15"/>
       <c r="X47" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="48" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="10" t="s">
+      <c r="D48" s="15"/>
+      <c r="E48" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="10" t="s">
+      <c r="F48" s="14"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I48" s="11"/>
-      <c r="J48" s="12"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="15"/>
       <c r="K48" s="3">
         <v>2</v>
       </c>
-      <c r="P48" s="10" t="s">
+      <c r="P48" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="Q48" s="12"/>
-      <c r="R48" s="10" t="s">
+      <c r="Q48" s="15"/>
+      <c r="R48" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S48" s="11"/>
-      <c r="T48" s="12"/>
-      <c r="U48" s="10" t="s">
+      <c r="S48" s="14"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="V48" s="11"/>
-      <c r="W48" s="12"/>
+      <c r="V48" s="14"/>
+      <c r="W48" s="15"/>
       <c r="X48" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="10" t="s">
+      <c r="D49" s="15"/>
+      <c r="E49" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="10" t="s">
+      <c r="F49" s="14"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="I49" s="11"/>
-      <c r="J49" s="12"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="15"/>
       <c r="K49" s="3">
         <v>1</v>
       </c>
-      <c r="P49" s="10" t="s">
+      <c r="P49" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="Q49" s="12"/>
-      <c r="R49" s="10" t="s">
+      <c r="Q49" s="15"/>
+      <c r="R49" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="S49" s="11"/>
-      <c r="T49" s="12"/>
-      <c r="U49" s="10" t="s">
+      <c r="S49" s="14"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="V49" s="11"/>
-      <c r="W49" s="12"/>
+      <c r="V49" s="14"/>
+      <c r="W49" s="15"/>
       <c r="X49" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="10" t="s">
+      <c r="D50" s="15"/>
+      <c r="E50" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F50" s="11"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="10" t="s">
+      <c r="F50" s="14"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I50" s="11"/>
-      <c r="J50" s="12"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="15"/>
       <c r="K50" s="3">
         <v>2</v>
       </c>
-      <c r="P50" s="10" t="s">
+      <c r="P50" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="Q50" s="12"/>
-      <c r="R50" s="10" t="s">
+      <c r="Q50" s="15"/>
+      <c r="R50" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="S50" s="11"/>
-      <c r="T50" s="12"/>
-      <c r="U50" s="10" t="s">
+      <c r="S50" s="14"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V50" s="11"/>
-      <c r="W50" s="12"/>
+      <c r="V50" s="14"/>
+      <c r="W50" s="15"/>
       <c r="X50" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="10" t="s">
+      <c r="D51" s="15"/>
+      <c r="E51" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="10" t="s">
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="I51" s="11"/>
-      <c r="J51" s="12"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="15"/>
       <c r="K51" s="3">
         <v>2</v>
       </c>
-      <c r="P51" s="10" t="s">
+      <c r="P51" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="Q51" s="12"/>
-      <c r="R51" s="10" t="s">
+      <c r="Q51" s="15"/>
+      <c r="R51" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="S51" s="11"/>
-      <c r="T51" s="12"/>
-      <c r="U51" s="10" t="s">
+      <c r="S51" s="14"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="V51" s="11"/>
-      <c r="W51" s="12"/>
+      <c r="V51" s="14"/>
+      <c r="W51" s="15"/>
       <c r="X51" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="10" t="s">
+      <c r="D52" s="15"/>
+      <c r="E52" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F52" s="11"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="10" t="s">
+      <c r="F52" s="14"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I52" s="11"/>
-      <c r="J52" s="12"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="15"/>
       <c r="K52" s="3">
         <v>5</v>
       </c>
-      <c r="P52" s="10" t="s">
+      <c r="P52" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="Q52" s="12"/>
-      <c r="R52" s="10" t="s">
+      <c r="Q52" s="15"/>
+      <c r="R52" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="S52" s="11"/>
-      <c r="T52" s="12"/>
-      <c r="U52" s="10" t="s">
+      <c r="S52" s="14"/>
+      <c r="T52" s="15"/>
+      <c r="U52" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="V52" s="11"/>
-      <c r="W52" s="12"/>
+      <c r="V52" s="14"/>
+      <c r="W52" s="15"/>
       <c r="X52" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="10" t="s">
+      <c r="D53" s="15"/>
+      <c r="E53" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F53" s="11"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="10" t="s">
+      <c r="F53" s="14"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I53" s="11"/>
-      <c r="J53" s="12"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="15"/>
       <c r="K53" s="3">
         <v>1</v>
       </c>
-      <c r="P53" s="10" t="s">
+      <c r="P53" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="10" t="s">
+      <c r="Q53" s="15"/>
+      <c r="R53" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="S53" s="11"/>
-      <c r="T53" s="12"/>
-      <c r="U53" s="10" t="s">
+      <c r="S53" s="14"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="V53" s="11"/>
-      <c r="W53" s="12"/>
+      <c r="V53" s="14"/>
+      <c r="W53" s="15"/>
       <c r="X53" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="10" t="s">
+      <c r="D54" s="15"/>
+      <c r="E54" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="10" t="s">
+      <c r="F54" s="14"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I54" s="11"/>
-      <c r="J54" s="12"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="15"/>
       <c r="K54" s="3">
         <v>3</v>
       </c>
-      <c r="P54" s="10" t="s">
+      <c r="P54" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="Q54" s="12"/>
-      <c r="R54" s="10" t="s">
+      <c r="Q54" s="15"/>
+      <c r="R54" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="S54" s="11"/>
-      <c r="T54" s="12"/>
-      <c r="U54" s="10" t="s">
+      <c r="S54" s="14"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V54" s="11"/>
-      <c r="W54" s="12"/>
+      <c r="V54" s="14"/>
+      <c r="W54" s="15"/>
       <c r="X54" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="55" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="10" t="s">
+      <c r="D55" s="15"/>
+      <c r="E55" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F55" s="11"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="10" t="s">
+      <c r="F55" s="14"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="I55" s="11"/>
-      <c r="J55" s="12"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="15"/>
       <c r="K55" s="3">
         <v>1</v>
       </c>
-      <c r="P55" s="10" t="s">
+      <c r="P55" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="10" t="s">
+      <c r="Q55" s="15"/>
+      <c r="R55" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="S55" s="11"/>
-      <c r="T55" s="12"/>
-      <c r="U55" s="10" t="s">
+      <c r="S55" s="14"/>
+      <c r="T55" s="15"/>
+      <c r="U55" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="V55" s="11"/>
-      <c r="W55" s="12"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="15"/>
       <c r="X55" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="10" t="s">
+      <c r="D56" s="15"/>
+      <c r="E56" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="11"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="10" t="s">
+      <c r="F56" s="14"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I56" s="11"/>
-      <c r="J56" s="12"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="15"/>
       <c r="K56" s="3">
         <v>1</v>
       </c>
-      <c r="P56" s="10" t="s">
+      <c r="P56" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="10" t="s">
+      <c r="Q56" s="15"/>
+      <c r="R56" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="S56" s="11"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="10" t="s">
+      <c r="S56" s="14"/>
+      <c r="T56" s="15"/>
+      <c r="U56" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="V56" s="11"/>
-      <c r="W56" s="12"/>
+      <c r="V56" s="14"/>
+      <c r="W56" s="15"/>
       <c r="X56" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="10" t="s">
+      <c r="D57" s="15"/>
+      <c r="E57" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F57" s="11"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="10" t="s">
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="I57" s="11"/>
-      <c r="J57" s="12"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="15"/>
       <c r="K57" s="3">
         <v>1</v>
       </c>
-      <c r="P57" s="10" t="s">
+      <c r="P57" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="10" t="s">
+      <c r="Q57" s="15"/>
+      <c r="R57" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="S57" s="11"/>
-      <c r="T57" s="12"/>
-      <c r="U57" s="10" t="s">
+      <c r="S57" s="14"/>
+      <c r="T57" s="15"/>
+      <c r="U57" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="V57" s="11"/>
-      <c r="W57" s="12"/>
+      <c r="V57" s="14"/>
+      <c r="W57" s="15"/>
       <c r="X57" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="D58" s="12"/>
-      <c r="E58" s="10" t="s">
+      <c r="D58" s="15"/>
+      <c r="E58" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F58" s="11"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="10" t="s">
+      <c r="F58" s="14"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I58" s="11"/>
-      <c r="J58" s="12"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="15"/>
       <c r="K58" s="3">
         <v>2</v>
       </c>
-      <c r="P58" s="10" t="s">
+      <c r="P58" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="10" t="s">
+      <c r="Q58" s="15"/>
+      <c r="R58" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="S58" s="11"/>
-      <c r="T58" s="12"/>
-      <c r="U58" s="10" t="s">
+      <c r="S58" s="14"/>
+      <c r="T58" s="15"/>
+      <c r="U58" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="V58" s="11"/>
-      <c r="W58" s="12"/>
+      <c r="V58" s="14"/>
+      <c r="W58" s="15"/>
       <c r="X58" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="10" t="s">
+      <c r="D59" s="15"/>
+      <c r="E59" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F59" s="11"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="10" t="s">
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="I59" s="11"/>
-      <c r="J59" s="12"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="15"/>
       <c r="K59" s="3">
         <v>1</v>
       </c>
-      <c r="P59" s="10" t="s">
+      <c r="P59" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="Q59" s="12"/>
-      <c r="R59" s="10" t="s">
+      <c r="Q59" s="15"/>
+      <c r="R59" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="S59" s="11"/>
-      <c r="T59" s="12"/>
-      <c r="U59" s="10" t="s">
+      <c r="S59" s="14"/>
+      <c r="T59" s="15"/>
+      <c r="U59" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="V59" s="11"/>
-      <c r="W59" s="12"/>
+      <c r="V59" s="14"/>
+      <c r="W59" s="15"/>
       <c r="X59" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="60" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="10" t="s">
+      <c r="D60" s="15"/>
+      <c r="E60" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F60" s="11"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="10" t="s">
+      <c r="F60" s="14"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I60" s="11"/>
-      <c r="J60" s="12"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="15"/>
       <c r="K60" s="3">
         <v>1</v>
       </c>
-      <c r="P60" s="10" t="s">
+      <c r="P60" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="Q60" s="12"/>
-      <c r="R60" s="10" t="s">
+      <c r="Q60" s="15"/>
+      <c r="R60" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="S60" s="11"/>
-      <c r="T60" s="12"/>
-      <c r="U60" s="10" t="s">
+      <c r="S60" s="14"/>
+      <c r="T60" s="15"/>
+      <c r="U60" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="V60" s="11"/>
-      <c r="W60" s="12"/>
+      <c r="V60" s="14"/>
+      <c r="W60" s="15"/>
       <c r="X60" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="10" t="s">
+      <c r="D61" s="15"/>
+      <c r="E61" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="10" t="s">
+      <c r="F61" s="14"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I61" s="11"/>
-      <c r="J61" s="12"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="15"/>
       <c r="K61" s="3">
         <v>4</v>
       </c>
-      <c r="P61" s="10" t="s">
+      <c r="P61" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="Q61" s="12"/>
-      <c r="R61" s="10" t="s">
+      <c r="Q61" s="15"/>
+      <c r="R61" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="S61" s="11"/>
-      <c r="T61" s="12"/>
-      <c r="U61" s="10" t="s">
+      <c r="S61" s="14"/>
+      <c r="T61" s="15"/>
+      <c r="U61" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="V61" s="11"/>
-      <c r="W61" s="12"/>
+      <c r="V61" s="14"/>
+      <c r="W61" s="15"/>
       <c r="X61" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="10" t="s">
+      <c r="D62" s="15"/>
+      <c r="E62" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F62" s="11"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="10" t="s">
+      <c r="F62" s="14"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="I62" s="11"/>
-      <c r="J62" s="12"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="15"/>
       <c r="K62" s="3">
         <v>2</v>
       </c>
-      <c r="P62" s="10" t="s">
+      <c r="P62" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="Q62" s="12"/>
-      <c r="R62" s="10" t="s">
+      <c r="Q62" s="15"/>
+      <c r="R62" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S62" s="11"/>
-      <c r="T62" s="12"/>
-      <c r="U62" s="10" t="s">
+      <c r="S62" s="14"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="V62" s="11"/>
-      <c r="W62" s="12"/>
+      <c r="V62" s="14"/>
+      <c r="W62" s="15"/>
       <c r="X62" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="10" t="s">
+      <c r="D63" s="15"/>
+      <c r="E63" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="F63" s="11"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="10" t="s">
+      <c r="F63" s="14"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="I63" s="11"/>
-      <c r="J63" s="12"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="15"/>
       <c r="K63" s="3">
         <v>6</v>
       </c>
-      <c r="P63" s="10" t="s">
+      <c r="P63" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="Q63" s="12"/>
-      <c r="R63" s="10" t="s">
+      <c r="Q63" s="15"/>
+      <c r="R63" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="S63" s="11"/>
-      <c r="T63" s="12"/>
-      <c r="U63" s="10" t="s">
+      <c r="S63" s="14"/>
+      <c r="T63" s="15"/>
+      <c r="U63" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="V63" s="11"/>
-      <c r="W63" s="12"/>
+      <c r="V63" s="14"/>
+      <c r="W63" s="15"/>
       <c r="X63" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D64" s="12"/>
-      <c r="E64" s="10" t="s">
+      <c r="D64" s="15"/>
+      <c r="E64" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F64" s="11"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="10" t="s">
+      <c r="F64" s="14"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I64" s="11"/>
-      <c r="J64" s="12"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="15"/>
       <c r="K64" s="3">
         <v>1</v>
       </c>
-      <c r="P64" s="10" t="s">
+      <c r="P64" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="Q64" s="12"/>
-      <c r="R64" s="10" t="s">
+      <c r="Q64" s="15"/>
+      <c r="R64" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="S64" s="11"/>
-      <c r="T64" s="12"/>
-      <c r="U64" s="10" t="s">
+      <c r="S64" s="14"/>
+      <c r="T64" s="15"/>
+      <c r="U64" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="V64" s="11"/>
-      <c r="W64" s="12"/>
+      <c r="V64" s="14"/>
+      <c r="W64" s="15"/>
       <c r="X64" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="65" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="10" t="s">
+      <c r="D65" s="15"/>
+      <c r="E65" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F65" s="11"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="10" t="s">
+      <c r="F65" s="14"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="I65" s="11"/>
-      <c r="J65" s="12"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="15"/>
       <c r="K65" s="3">
         <v>1</v>
       </c>
-      <c r="P65" s="10" t="s">
+      <c r="P65" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="Q65" s="12"/>
-      <c r="R65" s="10" t="s">
+      <c r="Q65" s="15"/>
+      <c r="R65" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="S65" s="11"/>
-      <c r="T65" s="12"/>
-      <c r="U65" s="10" t="s">
+      <c r="S65" s="14"/>
+      <c r="T65" s="15"/>
+      <c r="U65" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="V65" s="11"/>
-      <c r="W65" s="12"/>
+      <c r="V65" s="14"/>
+      <c r="W65" s="15"/>
       <c r="X65" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="66" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="10" t="s">
+      <c r="D66" s="15"/>
+      <c r="E66" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="10" t="s">
+      <c r="F66" s="14"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I66" s="11"/>
-      <c r="J66" s="12"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="15"/>
       <c r="K66" s="3">
         <v>1</v>
       </c>
-      <c r="P66" s="10" t="s">
+      <c r="P66" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="Q66" s="12"/>
-      <c r="R66" s="10" t="s">
+      <c r="Q66" s="15"/>
+      <c r="R66" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="S66" s="11"/>
-      <c r="T66" s="12"/>
-      <c r="U66" s="10" t="s">
+      <c r="S66" s="14"/>
+      <c r="T66" s="15"/>
+      <c r="U66" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="V66" s="11"/>
-      <c r="W66" s="12"/>
+      <c r="V66" s="14"/>
+      <c r="W66" s="15"/>
       <c r="X66" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="67" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D67" s="12"/>
-      <c r="E67" s="10" t="s">
+      <c r="D67" s="15"/>
+      <c r="E67" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F67" s="11"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="10" t="s">
+      <c r="F67" s="14"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I67" s="11"/>
-      <c r="J67" s="12"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="15"/>
       <c r="K67" s="3">
         <v>2</v>
       </c>
-      <c r="P67" s="10" t="s">
+      <c r="P67" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="Q67" s="11"/>
-      <c r="R67" s="11"/>
-      <c r="S67" s="11"/>
-      <c r="T67" s="11"/>
-      <c r="U67" s="11"/>
-      <c r="V67" s="11"/>
-      <c r="W67" s="12"/>
+      <c r="Q67" s="14"/>
+      <c r="R67" s="14"/>
+      <c r="S67" s="14"/>
+      <c r="T67" s="14"/>
+      <c r="U67" s="14"/>
+      <c r="V67" s="14"/>
+      <c r="W67" s="15"/>
       <c r="X67" s="3">
         <v>58</v>
       </c>
     </row>
     <row r="68" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="10" t="s">
+      <c r="D68" s="15"/>
+      <c r="E68" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F68" s="11"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="10" t="s">
+      <c r="F68" s="14"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="I68" s="11"/>
-      <c r="J68" s="12"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="15"/>
       <c r="K68" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="69" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D69" s="12"/>
-      <c r="E69" s="10" t="s">
+      <c r="D69" s="15"/>
+      <c r="E69" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F69" s="11"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="10" t="s">
+      <c r="F69" s="14"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="I69" s="11"/>
-      <c r="J69" s="12"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="15"/>
       <c r="K69" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="70" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D70" s="12"/>
-      <c r="E70" s="10" t="s">
+      <c r="D70" s="15"/>
+      <c r="E70" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F70" s="11"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="10" t="s">
+      <c r="F70" s="14"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="I70" s="11"/>
-      <c r="J70" s="12"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="15"/>
       <c r="K70" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C71" s="10" t="s">
+      <c r="C71" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="12"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="15"/>
       <c r="K71" s="3">
         <v>58</v>
       </c>
     </row>
     <row r="72" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C72" s="14" t="s">
+      <c r="C72" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
     </row>
     <row r="73" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
     </row>
     <row r="74" spans="3:24" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="C74" s="15" t="s">
+      <c r="C74" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D74" s="16"/>
-      <c r="E74" s="15" t="s">
+      <c r="D74" s="19"/>
+      <c r="E74" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F74" s="17"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="15" t="s">
+      <c r="F74" s="20"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I74" s="17"/>
-      <c r="J74" s="16"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="19"/>
       <c r="K74" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="12"/>
-      <c r="E75" s="10" t="s">
+      <c r="D75" s="15"/>
+      <c r="E75" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F75" s="11"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="10" t="s">
+      <c r="F75" s="14"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I75" s="11"/>
-      <c r="J75" s="12"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="15"/>
       <c r="K75" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D76" s="12"/>
-      <c r="E76" s="10" t="s">
+      <c r="D76" s="15"/>
+      <c r="E76" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F76" s="11"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="10" t="s">
+      <c r="F76" s="14"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I76" s="11"/>
-      <c r="J76" s="12"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="15"/>
       <c r="K76" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C77" s="10" t="s">
+      <c r="C77" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D77" s="12"/>
-      <c r="E77" s="10" t="s">
+      <c r="D77" s="15"/>
+      <c r="E77" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F77" s="11"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="10" t="s">
+      <c r="F77" s="14"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I77" s="11"/>
-      <c r="J77" s="12"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="15"/>
       <c r="K77" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D78" s="12"/>
-      <c r="E78" s="10" t="s">
+      <c r="D78" s="15"/>
+      <c r="E78" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F78" s="11"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="10" t="s">
+      <c r="F78" s="14"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I78" s="11"/>
-      <c r="J78" s="12"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="15"/>
       <c r="K78" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="79" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C79" s="10" t="s">
+      <c r="C79" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D79" s="12"/>
-      <c r="E79" s="10" t="s">
+      <c r="D79" s="15"/>
+      <c r="E79" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F79" s="11"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="10" t="s">
+      <c r="F79" s="14"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I79" s="11"/>
-      <c r="J79" s="12"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="15"/>
       <c r="K79" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C80" s="10" t="s">
+      <c r="C80" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D80" s="12"/>
-      <c r="E80" s="10" t="s">
+      <c r="D80" s="15"/>
+      <c r="E80" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F80" s="11"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="10" t="s">
+      <c r="F80" s="14"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I80" s="11"/>
-      <c r="J80" s="12"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="15"/>
       <c r="K80" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="81" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D81" s="12"/>
-      <c r="E81" s="10" t="s">
+      <c r="D81" s="15"/>
+      <c r="E81" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F81" s="11"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="10" t="s">
+      <c r="F81" s="14"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I81" s="11"/>
-      <c r="J81" s="12"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="15"/>
       <c r="K81" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="82" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C82" s="10" t="s">
+      <c r="C82" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D82" s="12"/>
-      <c r="E82" s="10" t="s">
+      <c r="D82" s="15"/>
+      <c r="E82" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F82" s="11"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="10" t="s">
+      <c r="F82" s="14"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I82" s="11"/>
-      <c r="J82" s="12"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="15"/>
       <c r="K82" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="83" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D83" s="12"/>
-      <c r="E83" s="10" t="s">
+      <c r="D83" s="15"/>
+      <c r="E83" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F83" s="11"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="10" t="s">
+      <c r="F83" s="14"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I83" s="11"/>
-      <c r="J83" s="12"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="15"/>
       <c r="K83" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D84" s="12"/>
-      <c r="E84" s="10" t="s">
+      <c r="D84" s="15"/>
+      <c r="E84" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="11"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="10" t="s">
+      <c r="F84" s="14"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I84" s="11"/>
-      <c r="J84" s="12"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="15"/>
       <c r="K84" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="85" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C85" s="10" t="s">
+      <c r="C85" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D85" s="12"/>
-      <c r="E85" s="10" t="s">
+      <c r="D85" s="15"/>
+      <c r="E85" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F85" s="11"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="10" t="s">
+      <c r="F85" s="14"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I85" s="11"/>
-      <c r="J85" s="12"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="15"/>
       <c r="K85" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="86" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C86" s="10" t="s">
+      <c r="C86" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D86" s="12"/>
-      <c r="E86" s="10" t="s">
+      <c r="D86" s="15"/>
+      <c r="E86" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F86" s="11"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="10" t="s">
+      <c r="F86" s="14"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I86" s="11"/>
-      <c r="J86" s="12"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="15"/>
       <c r="K86" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C87" s="10" t="s">
+      <c r="C87" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D87" s="12"/>
-      <c r="E87" s="10" t="s">
+      <c r="D87" s="15"/>
+      <c r="E87" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F87" s="11"/>
-      <c r="G87" s="12"/>
-      <c r="H87" s="10" t="s">
+      <c r="F87" s="14"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I87" s="11"/>
-      <c r="J87" s="12"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="15"/>
       <c r="K87" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C88" s="10" t="s">
+      <c r="C88" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D88" s="12"/>
-      <c r="E88" s="10" t="s">
+      <c r="D88" s="15"/>
+      <c r="E88" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F88" s="11"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="10" t="s">
+      <c r="F88" s="14"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I88" s="11"/>
-      <c r="J88" s="12"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="15"/>
       <c r="K88" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="89" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C89" s="10" t="s">
+      <c r="C89" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D89" s="12"/>
-      <c r="E89" s="10" t="s">
+      <c r="D89" s="15"/>
+      <c r="E89" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F89" s="11"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="10" t="s">
+      <c r="F89" s="14"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I89" s="11"/>
-      <c r="J89" s="12"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="15"/>
       <c r="K89" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C90" s="10" t="s">
+      <c r="C90" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="12"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="15"/>
       <c r="K90" s="3">
         <v>34</v>
       </c>
     </row>
     <row r="91" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C91" s="14" t="s">
+      <c r="C91" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
+      <c r="D91" s="17"/>
+      <c r="E91" s="17"/>
+      <c r="F91" s="17"/>
     </row>
     <row r="92" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="16"/>
     </row>
     <row r="93" spans="3:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
     </row>
     <row r="94" spans="3:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D94" s="16"/>
-      <c r="E94" s="15" t="s">
+      <c r="D94" s="19"/>
+      <c r="E94" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F94" s="17"/>
-      <c r="G94" s="16"/>
-      <c r="H94" s="15" t="s">
+      <c r="F94" s="20"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I94" s="17"/>
-      <c r="J94" s="16"/>
+      <c r="I94" s="20"/>
+      <c r="J94" s="19"/>
       <c r="K94" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="95" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C95" s="10" t="s">
+      <c r="C95" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D95" s="12"/>
-      <c r="E95" s="10" t="s">
+      <c r="D95" s="15"/>
+      <c r="E95" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F95" s="11"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="10" t="s">
+      <c r="F95" s="14"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I95" s="11"/>
-      <c r="J95" s="12"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="15"/>
       <c r="K95" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C96" s="10" t="s">
+      <c r="C96" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D96" s="12"/>
-      <c r="E96" s="10" t="s">
+      <c r="D96" s="15"/>
+      <c r="E96" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="11"/>
-      <c r="G96" s="12"/>
-      <c r="H96" s="10" t="s">
+      <c r="F96" s="14"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I96" s="11"/>
-      <c r="J96" s="12"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="15"/>
       <c r="K96" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C97" s="10" t="s">
+      <c r="C97" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D97" s="12"/>
-      <c r="E97" s="10" t="s">
+      <c r="D97" s="15"/>
+      <c r="E97" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F97" s="11"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="10" t="s">
+      <c r="F97" s="14"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I97" s="11"/>
-      <c r="J97" s="12"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="15"/>
       <c r="K97" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="98" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C98" s="10" t="s">
+      <c r="C98" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D98" s="12"/>
-      <c r="E98" s="10" t="s">
+      <c r="D98" s="15"/>
+      <c r="E98" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F98" s="11"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="10" t="s">
+      <c r="F98" s="14"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I98" s="11"/>
-      <c r="J98" s="12"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="15"/>
       <c r="K98" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="99" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C99" s="10" t="s">
+      <c r="C99" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D99" s="12"/>
-      <c r="E99" s="10" t="s">
+      <c r="D99" s="15"/>
+      <c r="E99" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F99" s="11"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="10" t="s">
+      <c r="F99" s="14"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I99" s="11"/>
-      <c r="J99" s="12"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="15"/>
       <c r="K99" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="100" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C100" s="10" t="s">
+      <c r="C100" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D100" s="12"/>
-      <c r="E100" s="10" t="s">
+      <c r="D100" s="15"/>
+      <c r="E100" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F100" s="11"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="10" t="s">
+      <c r="F100" s="14"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I100" s="11"/>
-      <c r="J100" s="12"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="15"/>
       <c r="K100" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="101" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C101" s="10" t="s">
+      <c r="C101" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D101" s="12"/>
-      <c r="E101" s="10" t="s">
+      <c r="D101" s="15"/>
+      <c r="E101" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F101" s="11"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="10" t="s">
+      <c r="F101" s="14"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I101" s="11"/>
-      <c r="J101" s="12"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="15"/>
       <c r="K101" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="102" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C102" s="10" t="s">
+      <c r="C102" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D102" s="12"/>
-      <c r="E102" s="10" t="s">
+      <c r="D102" s="15"/>
+      <c r="E102" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F102" s="11"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="10" t="s">
+      <c r="F102" s="14"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="I102" s="11"/>
-      <c r="J102" s="12"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="15"/>
       <c r="K102" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="103" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C103" s="10" t="s">
+      <c r="C103" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D103" s="12"/>
-      <c r="E103" s="10" t="s">
+      <c r="D103" s="15"/>
+      <c r="E103" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F103" s="11"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="10" t="s">
+      <c r="F103" s="14"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I103" s="11"/>
-      <c r="J103" s="12"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="15"/>
       <c r="K103" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C104" s="10" t="s">
+      <c r="C104" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D104" s="12"/>
-      <c r="E104" s="10" t="s">
+      <c r="D104" s="15"/>
+      <c r="E104" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F104" s="11"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="10" t="s">
+      <c r="F104" s="14"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="I104" s="11"/>
-      <c r="J104" s="12"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="15"/>
       <c r="K104" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="105" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C105" s="10" t="s">
+      <c r="C105" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D105" s="12"/>
-      <c r="E105" s="10" t="s">
+      <c r="D105" s="15"/>
+      <c r="E105" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F105" s="11"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="10" t="s">
+      <c r="F105" s="14"/>
+      <c r="G105" s="15"/>
+      <c r="H105" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I105" s="11"/>
-      <c r="J105" s="12"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="15"/>
       <c r="K105" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C106" s="10" t="s">
+      <c r="C106" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D106" s="12"/>
-      <c r="E106" s="10" t="s">
+      <c r="D106" s="15"/>
+      <c r="E106" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F106" s="11"/>
-      <c r="G106" s="12"/>
-      <c r="H106" s="10" t="s">
+      <c r="F106" s="14"/>
+      <c r="G106" s="15"/>
+      <c r="H106" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I106" s="11"/>
-      <c r="J106" s="12"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="15"/>
       <c r="K106" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C107" s="10" t="s">
+      <c r="C107" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D107" s="12"/>
-      <c r="E107" s="10" t="s">
+      <c r="D107" s="15"/>
+      <c r="E107" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F107" s="11"/>
-      <c r="G107" s="12"/>
-      <c r="H107" s="10" t="s">
+      <c r="F107" s="14"/>
+      <c r="G107" s="15"/>
+      <c r="H107" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I107" s="11"/>
-      <c r="J107" s="12"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="15"/>
       <c r="K107" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C108" s="10" t="s">
+      <c r="C108" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D108" s="12"/>
-      <c r="E108" s="10" t="s">
+      <c r="D108" s="15"/>
+      <c r="E108" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F108" s="11"/>
-      <c r="G108" s="12"/>
-      <c r="H108" s="10" t="s">
+      <c r="F108" s="14"/>
+      <c r="G108" s="15"/>
+      <c r="H108" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I108" s="11"/>
-      <c r="J108" s="12"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="15"/>
       <c r="K108" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="109" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C109" s="10" t="s">
+      <c r="C109" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D109" s="12"/>
-      <c r="E109" s="10" t="s">
+      <c r="D109" s="15"/>
+      <c r="E109" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F109" s="11"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="10" t="s">
+      <c r="F109" s="14"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I109" s="11"/>
-      <c r="J109" s="12"/>
+      <c r="I109" s="14"/>
+      <c r="J109" s="15"/>
       <c r="K109" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C110" s="10" t="s">
+      <c r="C110" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="11"/>
-      <c r="J110" s="12"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="14"/>
+      <c r="I110" s="14"/>
+      <c r="J110" s="15"/>
       <c r="K110" s="3">
         <v>34</v>
       </c>
@@ -4609,5 +4699,6 @@
     <mergeCell ref="P65:Q65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>